<commit_message>
NoRecords Enhancement and Input Validation
</commit_message>
<xml_diff>
--- a/suppxls/Scen_demo_NoRecordsEnhancement_INS.xlsx
+++ b/suppxls/Scen_demo_NoRecordsEnhancement_INS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Model_Demo_Adv_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1633B46E-C332-4B47-B5A1-BD645FBD1A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CD4F4F-5E53-493B-B05C-CDAA09C3B53E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8400" yWindow="1425" windowWidth="28800" windowHeight="15345" xr2:uid="{26090C76-9FF4-4C7F-9A34-92857141728D}"/>
+    <workbookView xWindow="19090" yWindow="-9900" windowWidth="38620" windowHeight="21100" xr2:uid="{26090C76-9FF4-4C7F-9A34-92857141728D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="22">
   <si>
     <t>TFM_INS</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>~TFM_INS-TSL</t>
+  </si>
+  <si>
+    <t>dsadsadsad</t>
+  </si>
+  <si>
+    <t>dsadsad</t>
+  </si>
+  <si>
+    <t>ewqewq</t>
+  </si>
+  <si>
+    <t>fghfghfg</t>
   </si>
 </sst>
 </file>
@@ -512,7 +524,7 @@
   <dimension ref="B1:V31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,6 +729,9 @@
       <c r="S18">
         <v>0</v>
       </c>
+      <c r="T18" t="s">
+        <v>21</v>
+      </c>
       <c r="V18" t="s">
         <v>11</v>
       </c>
@@ -731,6 +746,9 @@
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
       <c r="F20">
         <v>2050</v>
       </c>
@@ -861,6 +879,9 @@
       <c r="S29" t="s">
         <v>11</v>
       </c>
+      <c r="T29" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="30" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
@@ -882,6 +903,9 @@
       </c>
       <c r="F31" t="s">
         <v>11</v>
+      </c>
+      <c r="H31" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>